<commit_message>
Fixed the algorithm a little bit
</commit_message>
<xml_diff>
--- a/excelMaker/results.xlsx
+++ b/excelMaker/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>Sample</t>
   </si>
@@ -62,6 +62,129 @@
   </si>
   <si>
     <t>EB9</t>
+  </si>
+  <si>
+    <t>EB10</t>
+  </si>
+  <si>
+    <t>EB11</t>
+  </si>
+  <si>
+    <t>EB12</t>
+  </si>
+  <si>
+    <t>EB13</t>
+  </si>
+  <si>
+    <t>EB14</t>
+  </si>
+  <si>
+    <t>EB15</t>
+  </si>
+  <si>
+    <t>EB16</t>
+  </si>
+  <si>
+    <t>EB17</t>
+  </si>
+  <si>
+    <t>EB18</t>
+  </si>
+  <si>
+    <t>EB19</t>
+  </si>
+  <si>
+    <t>EB20</t>
+  </si>
+  <si>
+    <t>EB21</t>
+  </si>
+  <si>
+    <t>EB22</t>
+  </si>
+  <si>
+    <t>EB23</t>
+  </si>
+  <si>
+    <t>EB24</t>
+  </si>
+  <si>
+    <t>EB25</t>
+  </si>
+  <si>
+    <t>EB26</t>
+  </si>
+  <si>
+    <t>EB27</t>
+  </si>
+  <si>
+    <t>EB28</t>
+  </si>
+  <si>
+    <t>EB29</t>
+  </si>
+  <si>
+    <t>EB30</t>
+  </si>
+  <si>
+    <t>EB31</t>
+  </si>
+  <si>
+    <t>EB32</t>
+  </si>
+  <si>
+    <t>EB33</t>
+  </si>
+  <si>
+    <t>EB34</t>
+  </si>
+  <si>
+    <t>EB35</t>
+  </si>
+  <si>
+    <t>EB36</t>
+  </si>
+  <si>
+    <t>EB37</t>
+  </si>
+  <si>
+    <t>EB38</t>
+  </si>
+  <si>
+    <t>EB39</t>
+  </si>
+  <si>
+    <t>EB40</t>
+  </si>
+  <si>
+    <t>EB41</t>
+  </si>
+  <si>
+    <t>EB42</t>
+  </si>
+  <si>
+    <t>EB43</t>
+  </si>
+  <si>
+    <t>EB44</t>
+  </si>
+  <si>
+    <t>EB45</t>
+  </si>
+  <si>
+    <t>EB46</t>
+  </si>
+  <si>
+    <t>EB47</t>
+  </si>
+  <si>
+    <t>EB48</t>
+  </si>
+  <si>
+    <t>EB49</t>
+  </si>
+  <si>
+    <t>EB50</t>
   </si>
 </sst>
 </file>
@@ -443,6 +566,1564 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="6600825"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="EB10.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="7334250"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="EB11.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="8067675"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="EB12.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="8801100"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="EB13.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="9534525"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="EB14.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="10267950"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="EB15.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="11001375"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="EB16.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="11734800"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17" descr="EB17.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="12468225"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18" descr="EB18.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="13201650"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19" descr="EB19.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="13935075"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20" descr="EB20.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="14668500"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21" descr="EB21.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="15401925"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22" descr="EB22.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="16135350"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23" descr="EB23.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="16868775"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24" descr="EB24.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="17602200"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25" descr="EB25.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="18335625"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26" descr="EB26.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="19069050"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27" descr="EB27.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="19802475"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28" descr="EB28.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="20535900"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29" descr="EB29.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="21269325"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30" descr="EB30.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="22002750"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31" descr="EB31.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="22736175"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32" descr="EB32.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="23469600"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33" descr="EB33.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="24203025"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34" descr="EB34.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="24936450"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35" descr="EB35.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="25669875"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36" descr="EB36.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="26403300"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37" descr="EB37.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="27136725"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38" descr="EB38.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="27870150"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39" descr="EB39.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="28603575"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40" descr="EB40.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="29337000"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41" descr="EB41.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="30070425"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42" descr="EB42.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="30803850"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43" descr="EB43.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="31537275"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44" descr="EB44.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="32270700"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45" descr="EB45.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="33004125"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46" descr="EB46.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="33737550"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47" descr="EB47.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="34470975"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48" descr="EB48.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="35204400"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49" descr="EB49.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="35937825"/>
+          <a:ext cx="731520" cy="731520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>731520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50" descr="EB50.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="36671250"/>
           <a:ext cx="731520" cy="731520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -740,7 +2421,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -922,6 +2603,703 @@
         <v>3.197067055623447</v>
       </c>
     </row>
+    <row r="11" spans="1:6" ht="58" customHeight="1">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>2093</v>
+      </c>
+      <c r="E11">
+        <v>30435</v>
+      </c>
+      <c r="F11">
+        <v>6.876950878922293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="58" customHeight="1">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>1249</v>
+      </c>
+      <c r="E12">
+        <v>32564</v>
+      </c>
+      <c r="F12">
+        <v>3.835523891413831</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="58" customHeight="1">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>1353</v>
+      </c>
+      <c r="E13">
+        <v>41685</v>
+      </c>
+      <c r="F13">
+        <v>3.245771860381432</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="58" customHeight="1">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>4652</v>
+      </c>
+      <c r="E14">
+        <v>24495</v>
+      </c>
+      <c r="F14">
+        <v>18.99163094509083</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="58" customHeight="1">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>1537</v>
+      </c>
+      <c r="E15">
+        <v>23639</v>
+      </c>
+      <c r="F15">
+        <v>6.501967088286306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="58" customHeight="1">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>6229</v>
+      </c>
+      <c r="E16">
+        <v>42890</v>
+      </c>
+      <c r="F16">
+        <v>14.52319888085801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="58" customHeight="1">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>2089</v>
+      </c>
+      <c r="E17">
+        <v>34148</v>
+      </c>
+      <c r="F17">
+        <v>6.117488579126157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="58" customHeight="1">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>919</v>
+      </c>
+      <c r="E18">
+        <v>46780</v>
+      </c>
+      <c r="F18">
+        <v>1.964514749893117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="58" customHeight="1">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>2116</v>
+      </c>
+      <c r="E19">
+        <v>30973</v>
+      </c>
+      <c r="F19">
+        <v>6.831756691311789</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="58" customHeight="1">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>2953</v>
+      </c>
+      <c r="E20">
+        <v>33518</v>
+      </c>
+      <c r="F20">
+        <v>8.810191538874633</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="58" customHeight="1">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>1083</v>
+      </c>
+      <c r="E21">
+        <v>31713</v>
+      </c>
+      <c r="F21">
+        <v>3.415003310945038</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="58" customHeight="1">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>8379</v>
+      </c>
+      <c r="E22">
+        <v>20112</v>
+      </c>
+      <c r="F22">
+        <v>41.66169451073986</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="58" customHeight="1">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>534</v>
+      </c>
+      <c r="E23">
+        <v>29433</v>
+      </c>
+      <c r="F23">
+        <v>1.814290082560392</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="58" customHeight="1">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>8410</v>
+      </c>
+      <c r="E24">
+        <v>29556</v>
+      </c>
+      <c r="F24">
+        <v>28.45445933143862</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="58" customHeight="1">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>2772</v>
+      </c>
+      <c r="E25">
+        <v>35801</v>
+      </c>
+      <c r="F25">
+        <v>7.742800480433508</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="58" customHeight="1">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>860</v>
+      </c>
+      <c r="E26">
+        <v>33092</v>
+      </c>
+      <c r="F26">
+        <v>2.598815423667352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="58" customHeight="1">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>3779</v>
+      </c>
+      <c r="E27">
+        <v>22440</v>
+      </c>
+      <c r="F27">
+        <v>16.84046345811052</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="58" customHeight="1">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>451</v>
+      </c>
+      <c r="E28">
+        <v>27505</v>
+      </c>
+      <c r="F28">
+        <v>1.639701872386839</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="58" customHeight="1">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>8043</v>
+      </c>
+      <c r="E29">
+        <v>38963</v>
+      </c>
+      <c r="F29">
+        <v>20.6426609860637</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="58" customHeight="1">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>492</v>
+      </c>
+      <c r="E30">
+        <v>28804</v>
+      </c>
+      <c r="F30">
+        <v>1.708096097764199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="58" customHeight="1">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>755</v>
+      </c>
+      <c r="E31">
+        <v>30941</v>
+      </c>
+      <c r="F31">
+        <v>2.44012798552083</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="58" customHeight="1">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>2114</v>
+      </c>
+      <c r="E32">
+        <v>34052</v>
+      </c>
+      <c r="F32">
+        <v>6.208152237754024</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="58" customHeight="1">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>7598</v>
+      </c>
+      <c r="E33">
+        <v>33433</v>
+      </c>
+      <c r="F33">
+        <v>22.72604911315168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="58" customHeight="1">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>734</v>
+      </c>
+      <c r="E34">
+        <v>31691</v>
+      </c>
+      <c r="F34">
+        <v>2.316114985327065</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="58" customHeight="1">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>1631</v>
+      </c>
+      <c r="E35">
+        <v>36203</v>
+      </c>
+      <c r="F35">
+        <v>4.505151506781206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="58" customHeight="1">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>3915</v>
+      </c>
+      <c r="E36">
+        <v>40223</v>
+      </c>
+      <c r="F36">
+        <v>9.733237202595529</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="58" customHeight="1">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <v>879</v>
+      </c>
+      <c r="E37">
+        <v>33187</v>
+      </c>
+      <c r="F37">
+        <v>2.648627474613554</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="58" customHeight="1">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>1787</v>
+      </c>
+      <c r="E38">
+        <v>31326</v>
+      </c>
+      <c r="F38">
+        <v>5.704526591329886</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="58" customHeight="1">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>7732</v>
+      </c>
+      <c r="E39">
+        <v>30538</v>
+      </c>
+      <c r="F39">
+        <v>25.31927434671557</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="58" customHeight="1">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40">
+        <v>1787</v>
+      </c>
+      <c r="E40">
+        <v>31326</v>
+      </c>
+      <c r="F40">
+        <v>5.704526591329886</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="58" customHeight="1">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>668</v>
+      </c>
+      <c r="E41">
+        <v>35115</v>
+      </c>
+      <c r="F41">
+        <v>1.902320945464901</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="58" customHeight="1">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <v>2179</v>
+      </c>
+      <c r="E42">
+        <v>29625</v>
+      </c>
+      <c r="F42">
+        <v>7.355274261603376</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="58" customHeight="1">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <v>2435</v>
+      </c>
+      <c r="E43">
+        <v>33158</v>
+      </c>
+      <c r="F43">
+        <v>7.34362748054768</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="58" customHeight="1">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>1172</v>
+      </c>
+      <c r="E44">
+        <v>28101</v>
+      </c>
+      <c r="F44">
+        <v>4.170670082915199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="58" customHeight="1">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>10420</v>
+      </c>
+      <c r="E45">
+        <v>31390</v>
+      </c>
+      <c r="F45">
+        <v>33.19528512265052</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="58" customHeight="1">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>2922</v>
+      </c>
+      <c r="E46">
+        <v>33313</v>
+      </c>
+      <c r="F46">
+        <v>8.77135052381953</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="58" customHeight="1">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>4185</v>
+      </c>
+      <c r="E47">
+        <v>27752</v>
+      </c>
+      <c r="F47">
+        <v>15.07999423464975</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="58" customHeight="1">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>1014</v>
+      </c>
+      <c r="E48">
+        <v>24963</v>
+      </c>
+      <c r="F48">
+        <v>4.062011777430597</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="58" customHeight="1">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>1881</v>
+      </c>
+      <c r="E49">
+        <v>33744</v>
+      </c>
+      <c r="F49">
+        <v>5.574324324324325</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="58" customHeight="1">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>7974</v>
+      </c>
+      <c r="E50">
+        <v>24731</v>
+      </c>
+      <c r="F50">
+        <v>32.24293396951195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="58" customHeight="1">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51">
+        <v>2870</v>
+      </c>
+      <c r="E51">
+        <v>40912</v>
+      </c>
+      <c r="F51">
+        <v>7.015056707078609</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>